<commit_message>
Info added in GitExcel1.xlsx
</commit_message>
<xml_diff>
--- a/GitExcel1.xlsx
+++ b/GitExcel1.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\A0833739\OneDrive - Aon\Desktop\Git Demo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://my.aon.net/personal/vikram_kumar_jha_aon_com/Documents/Desktop/Git Demo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D71A32F5-D36B-49EB-9C63-7C9C31506074}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{D71A32F5-D36B-49EB-9C63-7C9C31506074}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8E9FE343-F869-4899-B010-FB0A25A84726}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Name</t>
   </si>
@@ -34,6 +34,9 @@
   </si>
   <si>
     <t>Vikram Kumar Jha</t>
+  </si>
+  <si>
+    <t>Suraj Kumar Jha</t>
   </si>
 </sst>
 </file>
@@ -100,6 +103,13 @@
   </cellStyles>
   <dxfs count="3">
     <dxf>
+      <numFmt numFmtId="20" formatCode="d\-mmm\-yy"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -118,13 +128,6 @@
       </font>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
-    <dxf>
-      <numFmt numFmtId="20" formatCode="d\-mmm\-yy"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -139,11 +142,11 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{928C5268-BD81-48D0-A6AC-433954673FFB}" name="Table3" displayName="Table3" ref="A1:B13" totalsRowShown="0" headerRowDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{928C5268-BD81-48D0-A6AC-433954673FFB}" name="Table3" displayName="Table3" ref="A1:B13" totalsRowShown="0" headerRowDxfId="2">
   <autoFilter ref="A1:B13" xr:uid="{928C5268-BD81-48D0-A6AC-433954673FFB}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{6F33B925-64EB-4B76-ABB1-00665FDB6323}" name="Name" dataDxfId="2"/>
-    <tableColumn id="2" xr3:uid="{2CE9EB4A-9773-4EDD-A1B4-2C1351DD2B18}" name="DOB" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{6F33B925-64EB-4B76-ABB1-00665FDB6323}" name="Name" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{2CE9EB4A-9773-4EDD-A1B4-2C1351DD2B18}" name="DOB" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -415,7 +418,7 @@
   <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -440,9 +443,13 @@
         <v>36416</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A3" s="1"/>
-      <c r="B3" s="3"/>
+    <row r="3" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="3">
+        <v>36788</v>
+      </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" s="1"/>

</xml_diff>